<commit_message>
n_50 applied n_window partly missig
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48E7605-E323-4A00-969F-9357DC98C410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
@@ -153,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -547,16 +548,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -570,12 +571,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -584,12 +585,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -598,7 +599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -615,16 +616,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -638,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -652,7 +653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -666,7 +667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -680,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -700,20 +701,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -727,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -741,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -755,7 +756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -775,33 +776,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3046875" customWidth="1"/>
+    <col min="6" max="6" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.3046875" customWidth="1"/>
+    <col min="9" max="9" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3046875" customWidth="1"/>
+    <col min="12" max="12" width="14.3828125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C1" s="14" t="s">
         <v>35</v>
       </c>
@@ -819,7 +820,7 @@
       <c r="M1" s="14"/>
       <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C2" t="s">
         <v>36</v>
       </c>
@@ -857,7 +858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>33</v>
@@ -902,7 +903,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -949,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -996,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
         <v>7</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="10">
         <v>11</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
         <v>13</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" s="10">
         <v>15</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20" s="10">
         <v>17</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
         <v>19</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" s="10">
         <v>21</v>
       </c>
@@ -1889,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="13">
         <v>25</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -2124,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" s="10">
         <v>27</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -2218,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" s="10">
         <v>29</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A34" s="13">
         <v>31</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A36" s="10">
         <v>33</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A38" s="10">
         <v>35</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
         <v>36</v>
       </c>

</xml_diff>